<commit_message>
update codes and add more objects to branch
</commit_message>
<xml_diff>
--- a/ExperimentDesign/CNNwithSTFT_ExperimentDesign.xlsx
+++ b/ExperimentDesign/CNNwithSTFT_ExperimentDesign.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FRA-UAS\semester2\CompInt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FRA-UAS\semester2\CompInt\Code\CompInt-Project-T3\ExperimentDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF91EED-114F-42E4-B097-AA35C0D9D171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03613EE8-B9E9-4A9E-93C3-4871314E96B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F4F0541-79DD-4112-8FFC-CE99E882B6FB}"/>
   </bookViews>
@@ -63,10 +63,10 @@
     <t>Model</t>
   </si>
   <si>
-    <t>Second Phase : Testing</t>
+    <t>First Phase : Training</t>
   </si>
   <si>
-    <t>First Phase : Training</t>
+    <t>Second Phase : Testing (Validation)</t>
   </si>
 </sst>
 </file>
@@ -187,14 +187,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>34020</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>180750</xdr:rowOff>
     </xdr:to>
@@ -231,20 +231,25 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>34020</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>23358</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -281,19 +286,24 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>574836</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>184461</xdr:rowOff>
@@ -331,20 +341,25 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>37485</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>184461</xdr:rowOff>
     </xdr:to>
@@ -381,19 +396,24 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>574837</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>180750</xdr:rowOff>
@@ -437,13 +457,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>574837</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>180750</xdr:rowOff>
@@ -487,13 +507,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>574837</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>180750</xdr:rowOff>
@@ -537,13 +557,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>574837</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>180750</xdr:rowOff>
@@ -587,14 +607,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>231321</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>158846</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>57941</xdr:colOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>57942</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>149679</xdr:rowOff>
     </xdr:to>
@@ -648,13 +668,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>44</xdr:col>
+      <xdr:col>46</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>50</xdr:col>
+      <xdr:col>52</xdr:col>
       <xdr:colOff>554182</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>103909</xdr:rowOff>
@@ -716,13 +736,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>398319</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>86591</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>155864</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>34636</xdr:rowOff>
@@ -780,13 +800,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>412173</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>100445</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>169719</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>48490</xdr:rowOff>
@@ -844,13 +864,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>99035</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>99035</xdr:rowOff>
@@ -903,13 +923,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>99035</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>124248</xdr:rowOff>
@@ -962,13 +982,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>99035</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>100890</xdr:rowOff>
@@ -1021,13 +1041,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>574836</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>99034</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>100889</xdr:rowOff>
@@ -1080,13 +1100,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>574837</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>154263</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>231321</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>99035</xdr:rowOff>
@@ -1139,13 +1159,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>574837</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>154263</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>231321</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>99034</xdr:rowOff>
@@ -1198,13 +1218,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>574837</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>99035</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>231321</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>154263</xdr:rowOff>
@@ -1257,13 +1277,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>574837</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>99035</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>231321</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>154263</xdr:rowOff>
@@ -1316,13 +1336,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>40</xdr:col>
+      <xdr:col>42</xdr:col>
       <xdr:colOff>57941</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>154263</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>44</xdr:col>
+      <xdr:col>46</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>155864</xdr:rowOff>
@@ -1375,13 +1395,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>79</xdr:row>
       <xdr:rowOff>21648</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>554183</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1444,15 +1464,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>367392</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>329046</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>311725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>90301</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>294408</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1467,8 +1487,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="605118" y="3003176"/>
-          <a:ext cx="3392980" cy="2487706"/>
+          <a:off x="935182" y="2892134"/>
+          <a:ext cx="3398074" cy="1714501"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1504,38 +1524,19 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="2000"/>
-            <a:t>Each Object has 315 Signals. We will</a:t>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="2000"/>
+            <a:t>INPUT</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000"/>
-            <a:t>train</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000" baseline="0"/>
-            <a:t> with</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000"/>
-            <a:t> 211 Signals, and use the rest for Testing.</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="2000"/>
-          </a:br>
-          <a:br>
-            <a:rPr lang="en-US" sz="2000"/>
-          </a:br>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" altLang="ja-JP" sz="2000"/>
-            <a:t>※ 67</a:t>
+            <a:t>※ 80</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="ja-JP" sz="2000" baseline="0"/>
-            <a:t> Percent for Training and 33 Percent for Testing</a:t>
+            <a:t> Percent for Training and 20 Percent for Testing</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="2000"/>
         </a:p>
@@ -1545,13 +1546,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>277091</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1607,7 +1608,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="2800"/>
-            <a:t>211</a:t>
+            <a:t>315</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1616,13 +1617,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>277091</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1678,7 +1679,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="2800"/>
-            <a:t>211</a:t>
+            <a:t>200</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1687,13 +1688,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>277091</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1749,7 +1750,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="2800"/>
-            <a:t>211</a:t>
+            <a:t>400</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1758,13 +1759,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>190501</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>277091</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>190501</xdr:rowOff>
@@ -1820,7 +1821,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="2800"/>
-            <a:t>211</a:t>
+            <a:t>m</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1829,7 +1830,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>34020</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1868,13 +1869,18 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>34020</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>23358</xdr:rowOff>
@@ -1913,13 +1919,18 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>113</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1958,13 +1969,18 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>37485</xdr:colOff>
       <xdr:row>95</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2003,13 +2019,18 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2054,7 +2075,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2099,7 +2120,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>95</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2144,7 +2165,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>113</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2189,13 +2210,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>398319</xdr:colOff>
       <xdr:row>105</xdr:row>
       <xdr:rowOff>86591</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>155864</xdr:colOff>
       <xdr:row>112</xdr:row>
       <xdr:rowOff>34636</xdr:rowOff>
@@ -2253,13 +2274,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>412173</xdr:colOff>
       <xdr:row>105</xdr:row>
       <xdr:rowOff>100445</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>169719</xdr:colOff>
       <xdr:row>112</xdr:row>
       <xdr:rowOff>48490</xdr:rowOff>
@@ -2317,13 +2338,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>51955</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>67644</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>67644</xdr:rowOff>
@@ -2376,13 +2397,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>51955</xdr:colOff>
       <xdr:row>86</xdr:row>
       <xdr:rowOff>67645</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>86</xdr:row>
       <xdr:rowOff>84199</xdr:rowOff>
@@ -2435,13 +2456,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>51955</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>67644</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>69500</xdr:rowOff>
@@ -2494,13 +2515,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>7666</xdr:colOff>
       <xdr:row>115</xdr:row>
       <xdr:rowOff>67646</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>115</xdr:row>
       <xdr:rowOff>69501</xdr:rowOff>
@@ -2553,13 +2574,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>277091</xdr:colOff>
       <xdr:row>79</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2615,7 +2636,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="2800"/>
-            <a:t>104</a:t>
+            <a:t>//</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2624,13 +2645,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>86</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>277091</xdr:colOff>
       <xdr:row>90</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2686,7 +2707,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="2800"/>
-            <a:t>104</a:t>
+            <a:t>//</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2695,13 +2716,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>277091</xdr:colOff>
       <xdr:row>101</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2757,7 +2778,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="2800"/>
-            <a:t>104</a:t>
+            <a:t>//</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2766,13 +2787,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>114</xdr:row>
       <xdr:rowOff>190501</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>277091</xdr:colOff>
       <xdr:row>118</xdr:row>
       <xdr:rowOff>190501</xdr:rowOff>
@@ -2828,7 +2849,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="2800"/>
-            <a:t>104</a:t>
+            <a:t>mm</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2837,13 +2858,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>129342</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>131197</xdr:rowOff>
@@ -2893,13 +2914,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>47080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>47080</xdr:rowOff>
@@ -2949,13 +2970,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>7667</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>67644</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>10824</xdr:rowOff>
@@ -3008,13 +3029,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>34</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>554183</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>17318</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
+      <xdr:col>42</xdr:col>
       <xdr:colOff>34636</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>10824</xdr:rowOff>
@@ -3066,13 +3087,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>7667</xdr:colOff>
       <xdr:row>86</xdr:row>
       <xdr:rowOff>67645</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>10824</xdr:rowOff>
@@ -3125,13 +3146,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>7667</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>10824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>67644</xdr:rowOff>
@@ -3184,13 +3205,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>7667</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>10824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>115</xdr:row>
       <xdr:rowOff>67646</xdr:rowOff>
@@ -3243,13 +3264,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>40</xdr:col>
+      <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
+      <xdr:col>47</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>80</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3336,13 +3357,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>40</xdr:col>
+      <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
+      <xdr:col>47</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>91</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3429,13 +3450,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>40</xdr:col>
+      <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>95</xdr:row>
       <xdr:rowOff>17318</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
+      <xdr:col>47</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>102</xdr:row>
       <xdr:rowOff>17318</xdr:rowOff>
@@ -3522,13 +3543,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>40</xdr:col>
+      <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>113</xdr:row>
       <xdr:rowOff>-1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
+      <xdr:col>47</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>120</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3615,13 +3636,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>34</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>554183</xdr:colOff>
       <xdr:row>86</xdr:row>
       <xdr:rowOff>121227</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
+      <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>10824</xdr:rowOff>
@@ -3674,13 +3695,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>34</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>554183</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>10824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
+      <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>138545</xdr:rowOff>
@@ -3733,13 +3754,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>34</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>588819</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>138545</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
+      <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>115</xdr:row>
       <xdr:rowOff>121227</xdr:rowOff>
@@ -3791,13 +3812,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>41</xdr:col>
+      <xdr:col>43</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>105</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>43</xdr:col>
+      <xdr:col>45</xdr:col>
       <xdr:colOff>376671</xdr:colOff>
       <xdr:row>111</xdr:row>
       <xdr:rowOff>138545</xdr:rowOff>
@@ -3855,13 +3876,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>47</xdr:col>
+      <xdr:col>49</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>50</xdr:col>
+      <xdr:col>52</xdr:col>
       <xdr:colOff>71437</xdr:colOff>
       <xdr:row>121</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -3918,13 +3939,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>50</xdr:col>
+      <xdr:col>52</xdr:col>
       <xdr:colOff>404812</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>71</xdr:col>
+      <xdr:col>73</xdr:col>
       <xdr:colOff>80826</xdr:colOff>
       <xdr:row>115</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
@@ -4277,399 +4298,399 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A403C48-F16A-4071-B8EA-3F4F6C55080D}">
-  <dimension ref="C2:AT123"/>
+  <dimension ref="E2:AV123"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="BH120" sqref="BH120"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:46" ht="92.25">
-      <c r="V2" s="6" t="s">
+    <row r="2" spans="5:48" ht="92.25">
+      <c r="X2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:46" s="7" customFormat="1" ht="33.75">
-      <c r="V3" s="8"/>
-    </row>
-    <row r="4" spans="3:46" ht="61.5">
-      <c r="C4" s="3" t="s">
-        <v>10</v>
+    <row r="3" spans="5:48" s="7" customFormat="1" ht="33.75">
+      <c r="X3" s="8"/>
+    </row>
+    <row r="4" spans="5:48" ht="61.5">
+      <c r="E4" s="3" t="s">
+        <v>9</v>
       </c>
-      <c r="V4" s="1"/>
-    </row>
-    <row r="5" spans="3:46" ht="33.75">
-      <c r="V5" s="1"/>
-    </row>
-    <row r="6" spans="3:46" ht="33.75">
-      <c r="V6" s="1"/>
-    </row>
-    <row r="7" spans="3:46" ht="33.75">
-      <c r="V7" s="1"/>
-    </row>
-    <row r="8" spans="3:46" ht="33.75">
-      <c r="V8" s="1"/>
-    </row>
-    <row r="9" spans="3:46" ht="61.5">
-      <c r="H9" s="2" t="s">
+      <c r="X4" s="1"/>
+    </row>
+    <row r="5" spans="5:48" ht="33.75">
+      <c r="X5" s="1"/>
+    </row>
+    <row r="6" spans="5:48" ht="33.75">
+      <c r="X6" s="1"/>
+    </row>
+    <row r="7" spans="5:48" ht="33.75">
+      <c r="X7" s="1"/>
+    </row>
+    <row r="8" spans="5:48" ht="33.75">
+      <c r="X8" s="1"/>
+    </row>
+    <row r="9" spans="5:48" ht="61.5">
+      <c r="J9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="2" t="s">
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
-      <c r="V9" s="3"/>
+      <c r="V9" s="2"/>
       <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
+      <c r="X9" s="3"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
-      <c r="AA9" s="2" t="s">
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AB9" s="2"/>
-      <c r="AT9" s="2" t="s">
+      <c r="AD9" s="2"/>
+      <c r="AV9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="3:46" ht="33.75">
-      <c r="V10" s="1"/>
-    </row>
-    <row r="13" spans="3:46" ht="46.5">
-      <c r="E13" s="5" t="s">
+    <row r="10" spans="5:48" ht="33.75">
+      <c r="X10" s="1"/>
+    </row>
+    <row r="13" spans="5:48" ht="46.5">
+      <c r="G13" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="3:46" ht="15.75">
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="3:46" ht="15.75">
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="3:46" ht="15.75">
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="5:5" ht="15.75">
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="5:5" ht="15.75">
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="5:5" ht="15.75">
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="5:5" ht="15.75">
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="5:5" ht="15.75">
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="5:5" ht="15.75">
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="5:5" ht="15.75">
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="5:5" ht="46.5">
-      <c r="E24" s="5" t="s">
+    <row r="14" spans="5:48" ht="15.75">
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="5:48" ht="15.75">
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="5:48" ht="15.75">
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="7:7" ht="15.75">
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="7:7" ht="15.75">
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="7:7" ht="15.75">
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="7:7" ht="15.75">
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="7:7" ht="15.75">
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="7:7" ht="15.75">
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="7:7" ht="15.75">
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="7:7" ht="46.5">
+      <c r="G24" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="5:5" ht="15.75">
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="5:5" ht="15.75">
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="5:5" ht="15.75">
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="5:5" ht="15.75">
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="5:5" ht="15.75">
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="5:5" ht="15.75">
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="5:5" ht="15.75">
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="5:5" ht="15.75">
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="5:5" ht="15.75">
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="5:5" ht="15.75">
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="5:5" ht="46.5">
-      <c r="E35" s="5" t="s">
+    <row r="25" spans="7:7" ht="15.75">
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="7:7" ht="15.75">
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="7:7" ht="15.75">
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="7:7" ht="15.75">
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="7:7" ht="15.75">
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="7:7" ht="15.75">
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="7:7" ht="15.75">
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="7:7" ht="15.75">
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="7:7" ht="15.75">
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="7:7" ht="15.75">
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="7:7" ht="46.5">
+      <c r="G35" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="5:5" ht="15.75">
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="5:5" ht="15.75">
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="5:5" ht="15.75">
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="5:5" ht="15.75">
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="5:5" ht="15.75">
-      <c r="E40" s="4"/>
-    </row>
-    <row r="41" spans="5:5" ht="15.75">
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="5:5" ht="15.75">
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="5:5" ht="15.75">
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="5:5" ht="15.75">
-      <c r="E44" s="4"/>
-    </row>
-    <row r="45" spans="5:5" ht="15.75">
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" spans="5:5" ht="15.75">
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" spans="5:5" ht="15.75">
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" spans="5:5" ht="15.75">
-      <c r="E48" s="4"/>
-    </row>
-    <row r="49" spans="5:5" ht="15.75">
-      <c r="E49" s="4"/>
-    </row>
-    <row r="50" spans="5:5" ht="15.75">
-      <c r="E50" s="4"/>
-    </row>
-    <row r="51" spans="5:5" ht="15.75">
-      <c r="E51" s="4"/>
-    </row>
-    <row r="52" spans="5:5" ht="15.75">
-      <c r="E52" s="4"/>
-    </row>
-    <row r="53" spans="5:5" ht="46.5">
-      <c r="E53" s="5" t="s">
+    <row r="36" spans="7:7" ht="15.75">
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="7:7" ht="15.75">
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="7:7" ht="15.75">
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="7:7" ht="15.75">
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="7:7" ht="15.75">
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="7:7" ht="15.75">
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="7:7" ht="15.75">
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="7:7" ht="15.75">
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" spans="7:7" ht="15.75">
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="7:7" ht="15.75">
+      <c r="G45" s="4"/>
+    </row>
+    <row r="46" spans="7:7" ht="15.75">
+      <c r="G46" s="4"/>
+    </row>
+    <row r="47" spans="7:7" ht="15.75">
+      <c r="G47" s="4"/>
+    </row>
+    <row r="48" spans="7:7" ht="15.75">
+      <c r="G48" s="4"/>
+    </row>
+    <row r="49" spans="7:7" ht="15.75">
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" spans="7:7" ht="15.75">
+      <c r="G50" s="4"/>
+    </row>
+    <row r="51" spans="7:7" ht="15.75">
+      <c r="G51" s="4"/>
+    </row>
+    <row r="52" spans="7:7" ht="15.75">
+      <c r="G52" s="4"/>
+    </row>
+    <row r="53" spans="7:7" ht="46.5">
+      <c r="G53" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="5:5" ht="15.75">
-      <c r="E54" s="4"/>
-    </row>
-    <row r="55" spans="5:5" ht="15.75">
-      <c r="E55" s="4"/>
-    </row>
-    <row r="56" spans="5:5" ht="15.75">
-      <c r="E56" s="4"/>
-    </row>
-    <row r="57" spans="5:5" ht="15.75">
-      <c r="E57" s="4"/>
-    </row>
-    <row r="58" spans="5:5" ht="15.75">
-      <c r="E58" s="4"/>
-    </row>
-    <row r="59" spans="5:5" ht="15.75">
-      <c r="E59" s="4"/>
-    </row>
-    <row r="60" spans="5:5" ht="15.75">
-      <c r="E60" s="4"/>
-    </row>
-    <row r="61" spans="5:5" ht="15.75">
-      <c r="E61" s="4"/>
-    </row>
-    <row r="62" spans="5:5" ht="15.75">
-      <c r="E62" s="4"/>
-    </row>
-    <row r="67" spans="3:5" s="7" customFormat="1"/>
-    <row r="68" spans="3:5" ht="61.5">
-      <c r="C68" s="3" t="s">
-        <v>9</v>
+    <row r="54" spans="7:7" ht="15.75">
+      <c r="G54" s="4"/>
+    </row>
+    <row r="55" spans="7:7" ht="15.75">
+      <c r="G55" s="4"/>
+    </row>
+    <row r="56" spans="7:7" ht="15.75">
+      <c r="G56" s="4"/>
+    </row>
+    <row r="57" spans="7:7" ht="15.75">
+      <c r="G57" s="4"/>
+    </row>
+    <row r="58" spans="7:7" ht="15.75">
+      <c r="G58" s="4"/>
+    </row>
+    <row r="59" spans="7:7" ht="15.75">
+      <c r="G59" s="4"/>
+    </row>
+    <row r="60" spans="7:7" ht="15.75">
+      <c r="G60" s="4"/>
+    </row>
+    <row r="61" spans="7:7" ht="15.75">
+      <c r="G61" s="4"/>
+    </row>
+    <row r="62" spans="7:7" ht="15.75">
+      <c r="G62" s="4"/>
+    </row>
+    <row r="67" spans="5:7" s="7" customFormat="1"/>
+    <row r="68" spans="5:7" ht="61.5">
+      <c r="E68" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="74" spans="3:5" ht="46.5">
-      <c r="E74" s="5" t="s">
+    <row r="74" spans="5:7" ht="46.5">
+      <c r="G74" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="3:5" ht="15.75">
-      <c r="E75" s="4"/>
-    </row>
-    <row r="76" spans="3:5" ht="15.75">
-      <c r="E76" s="4"/>
-    </row>
-    <row r="77" spans="3:5" ht="15.75">
-      <c r="E77" s="4"/>
-    </row>
-    <row r="78" spans="3:5" ht="15.75">
-      <c r="E78" s="4"/>
-    </row>
-    <row r="79" spans="3:5" ht="15.75">
-      <c r="E79" s="4"/>
-    </row>
-    <row r="80" spans="3:5" ht="15.75">
-      <c r="E80" s="4"/>
-    </row>
-    <row r="81" spans="5:5" ht="15.75">
-      <c r="E81" s="4"/>
-    </row>
-    <row r="82" spans="5:5" ht="15.75">
-      <c r="E82" s="4"/>
-    </row>
-    <row r="83" spans="5:5" ht="15.75">
-      <c r="E83" s="4"/>
-    </row>
-    <row r="84" spans="5:5" ht="15.75">
-      <c r="E84" s="4"/>
-    </row>
-    <row r="85" spans="5:5" ht="46.5">
-      <c r="E85" s="5" t="s">
+    <row r="75" spans="5:7" ht="15.75">
+      <c r="G75" s="4"/>
+    </row>
+    <row r="76" spans="5:7" ht="15.75">
+      <c r="G76" s="4"/>
+    </row>
+    <row r="77" spans="5:7" ht="15.75">
+      <c r="G77" s="4"/>
+    </row>
+    <row r="78" spans="5:7" ht="15.75">
+      <c r="G78" s="4"/>
+    </row>
+    <row r="79" spans="5:7" ht="15.75">
+      <c r="G79" s="4"/>
+    </row>
+    <row r="80" spans="5:7" ht="15.75">
+      <c r="G80" s="4"/>
+    </row>
+    <row r="81" spans="7:7" ht="15.75">
+      <c r="G81" s="4"/>
+    </row>
+    <row r="82" spans="7:7" ht="15.75">
+      <c r="G82" s="4"/>
+    </row>
+    <row r="83" spans="7:7" ht="15.75">
+      <c r="G83" s="4"/>
+    </row>
+    <row r="84" spans="7:7" ht="15.75">
+      <c r="G84" s="4"/>
+    </row>
+    <row r="85" spans="7:7" ht="46.5">
+      <c r="G85" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="5:5" ht="15.75">
-      <c r="E86" s="4"/>
-    </row>
-    <row r="87" spans="5:5" ht="15.75">
-      <c r="E87" s="4"/>
-    </row>
-    <row r="88" spans="5:5" ht="15.75">
-      <c r="E88" s="4"/>
-    </row>
-    <row r="89" spans="5:5" ht="15.75">
-      <c r="E89" s="4"/>
-    </row>
-    <row r="90" spans="5:5" ht="15.75">
-      <c r="E90" s="4"/>
-    </row>
-    <row r="91" spans="5:5" ht="15.75">
-      <c r="E91" s="4"/>
-    </row>
-    <row r="92" spans="5:5" ht="15.75">
-      <c r="E92" s="4"/>
-    </row>
-    <row r="93" spans="5:5" ht="15.75">
-      <c r="E93" s="4"/>
-    </row>
-    <row r="94" spans="5:5" ht="15.75">
-      <c r="E94" s="4"/>
-    </row>
-    <row r="95" spans="5:5" ht="15.75">
-      <c r="E95" s="4"/>
-    </row>
-    <row r="96" spans="5:5" ht="46.5">
-      <c r="E96" s="5" t="s">
+    <row r="86" spans="7:7" ht="15.75">
+      <c r="G86" s="4"/>
+    </row>
+    <row r="87" spans="7:7" ht="15.75">
+      <c r="G87" s="4"/>
+    </row>
+    <row r="88" spans="7:7" ht="15.75">
+      <c r="G88" s="4"/>
+    </row>
+    <row r="89" spans="7:7" ht="15.75">
+      <c r="G89" s="4"/>
+    </row>
+    <row r="90" spans="7:7" ht="15.75">
+      <c r="G90" s="4"/>
+    </row>
+    <row r="91" spans="7:7" ht="15.75">
+      <c r="G91" s="4"/>
+    </row>
+    <row r="92" spans="7:7" ht="15.75">
+      <c r="G92" s="4"/>
+    </row>
+    <row r="93" spans="7:7" ht="15.75">
+      <c r="G93" s="4"/>
+    </row>
+    <row r="94" spans="7:7" ht="15.75">
+      <c r="G94" s="4"/>
+    </row>
+    <row r="95" spans="7:7" ht="15.75">
+      <c r="G95" s="4"/>
+    </row>
+    <row r="96" spans="7:7" ht="46.5">
+      <c r="G96" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="5:5" ht="15.75">
-      <c r="E97" s="4"/>
-    </row>
-    <row r="98" spans="5:5" ht="15.75">
-      <c r="E98" s="4"/>
-    </row>
-    <row r="99" spans="5:5" ht="15.75">
-      <c r="E99" s="4"/>
-    </row>
-    <row r="100" spans="5:5" ht="15.75">
-      <c r="E100" s="4"/>
-    </row>
-    <row r="101" spans="5:5" ht="15.75">
-      <c r="E101" s="4"/>
-    </row>
-    <row r="102" spans="5:5" ht="15.75">
-      <c r="E102" s="4"/>
-    </row>
-    <row r="103" spans="5:5" ht="15.75">
-      <c r="E103" s="4"/>
-    </row>
-    <row r="104" spans="5:5" ht="15.75">
-      <c r="E104" s="4"/>
-    </row>
-    <row r="105" spans="5:5" ht="15.75">
-      <c r="E105" s="4"/>
-    </row>
-    <row r="106" spans="5:5" ht="15.75">
-      <c r="E106" s="4"/>
-    </row>
-    <row r="107" spans="5:5" ht="15.75">
-      <c r="E107" s="4"/>
-    </row>
-    <row r="108" spans="5:5" ht="15.75">
-      <c r="E108" s="4"/>
-    </row>
-    <row r="109" spans="5:5" ht="15.75">
-      <c r="E109" s="4"/>
-    </row>
-    <row r="110" spans="5:5" ht="15.75">
-      <c r="E110" s="4"/>
-    </row>
-    <row r="111" spans="5:5" ht="15.75">
-      <c r="E111" s="4"/>
-    </row>
-    <row r="112" spans="5:5" ht="15.75">
-      <c r="E112" s="4"/>
-    </row>
-    <row r="113" spans="5:5" ht="15.75">
-      <c r="E113" s="4"/>
-    </row>
-    <row r="114" spans="5:5" ht="46.5">
-      <c r="E114" s="5" t="s">
+    <row r="97" spans="7:7" ht="15.75">
+      <c r="G97" s="4"/>
+    </row>
+    <row r="98" spans="7:7" ht="15.75">
+      <c r="G98" s="4"/>
+    </row>
+    <row r="99" spans="7:7" ht="15.75">
+      <c r="G99" s="4"/>
+    </row>
+    <row r="100" spans="7:7" ht="15.75">
+      <c r="G100" s="4"/>
+    </row>
+    <row r="101" spans="7:7" ht="15.75">
+      <c r="G101" s="4"/>
+    </row>
+    <row r="102" spans="7:7" ht="15.75">
+      <c r="G102" s="4"/>
+    </row>
+    <row r="103" spans="7:7" ht="15.75">
+      <c r="G103" s="4"/>
+    </row>
+    <row r="104" spans="7:7" ht="15.75">
+      <c r="G104" s="4"/>
+    </row>
+    <row r="105" spans="7:7" ht="15.75">
+      <c r="G105" s="4"/>
+    </row>
+    <row r="106" spans="7:7" ht="15.75">
+      <c r="G106" s="4"/>
+    </row>
+    <row r="107" spans="7:7" ht="15.75">
+      <c r="G107" s="4"/>
+    </row>
+    <row r="108" spans="7:7" ht="15.75">
+      <c r="G108" s="4"/>
+    </row>
+    <row r="109" spans="7:7" ht="15.75">
+      <c r="G109" s="4"/>
+    </row>
+    <row r="110" spans="7:7" ht="15.75">
+      <c r="G110" s="4"/>
+    </row>
+    <row r="111" spans="7:7" ht="15.75">
+      <c r="G111" s="4"/>
+    </row>
+    <row r="112" spans="7:7" ht="15.75">
+      <c r="G112" s="4"/>
+    </row>
+    <row r="113" spans="7:7" ht="15.75">
+      <c r="G113" s="4"/>
+    </row>
+    <row r="114" spans="7:7" ht="46.5">
+      <c r="G114" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="5:5" ht="15.75">
-      <c r="E115" s="4"/>
-    </row>
-    <row r="116" spans="5:5" ht="15.75">
-      <c r="E116" s="4"/>
-    </row>
-    <row r="117" spans="5:5" ht="15.75">
-      <c r="E117" s="4"/>
-    </row>
-    <row r="118" spans="5:5" ht="15.75">
-      <c r="E118" s="4"/>
-    </row>
-    <row r="119" spans="5:5" ht="15.75">
-      <c r="E119" s="4"/>
-    </row>
-    <row r="120" spans="5:5" ht="15.75">
-      <c r="E120" s="4"/>
-    </row>
-    <row r="121" spans="5:5" ht="15.75">
-      <c r="E121" s="4"/>
-    </row>
-    <row r="122" spans="5:5" ht="15.75">
-      <c r="E122" s="4"/>
-    </row>
-    <row r="123" spans="5:5" ht="15.75">
-      <c r="E123" s="4"/>
+    <row r="115" spans="7:7" ht="15.75">
+      <c r="G115" s="4"/>
+    </row>
+    <row r="116" spans="7:7" ht="15.75">
+      <c r="G116" s="4"/>
+    </row>
+    <row r="117" spans="7:7" ht="15.75">
+      <c r="G117" s="4"/>
+    </row>
+    <row r="118" spans="7:7" ht="15.75">
+      <c r="G118" s="4"/>
+    </row>
+    <row r="119" spans="7:7" ht="15.75">
+      <c r="G119" s="4"/>
+    </row>
+    <row r="120" spans="7:7" ht="15.75">
+      <c r="G120" s="4"/>
+    </row>
+    <row r="121" spans="7:7" ht="15.75">
+      <c r="G121" s="4"/>
+    </row>
+    <row r="122" spans="7:7" ht="15.75">
+      <c r="G122" s="4"/>
+    </row>
+    <row r="123" spans="7:7" ht="15.75">
+      <c r="G123" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update delegate works in Python
</commit_message>
<xml_diff>
--- a/ExperimentDesign/CNNwithSTFT_ExperimentDesign.xlsx
+++ b/ExperimentDesign/CNNwithSTFT_ExperimentDesign.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FRA-UAS\semester2\CompInt\Code\CompInt-Project-T3\ExperimentDesign\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FRA-UAS\semester2\CompInt\CompInt-Project-T3\ExperimentDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03613EE8-B9E9-4A9E-93C3-4871314E96B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE325C6-C4EB-4355-BFD2-4E838B43AA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F4F0541-79DD-4112-8FFC-CE99E882B6FB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Experiment Design" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t xml:space="preserve">CNN with STFT Experiment Design </t>
   </si>
@@ -68,12 +68,18 @@
   <si>
     <t>Second Phase : Testing (Validation)</t>
   </si>
+  <si>
+    <t>Migrate to Python</t>
+  </si>
+  <si>
+    <t>2 Parts</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,8 +135,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,6 +154,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -156,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -166,6 +186,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3996,6 +4018,669 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>363683</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>17319</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18D8945E-E663-4F46-A27B-30694D8B508F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3030682" y="36437454"/>
+          <a:ext cx="4000501" cy="4000501"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="3600">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Preprocessing</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>363683</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>17319</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="Rectangle: Rounded Corners 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6DFBB21-FA68-402D-B8D9-3698770A1425}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12728864" y="36437454"/>
+          <a:ext cx="4000501" cy="4000501"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="3600">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>CNN Training and Validation</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>259772</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CB35B9F-40E8-48A7-8D7C-6197087B232C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7273636" y="36420136"/>
+          <a:ext cx="3896591" cy="4017818"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>- Transform</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> csv files from each object into Spectrogram</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>- Able to change the following parameters </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>1. Window type</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>2. Window size</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>3. Overlapped</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>- Also be able to  downsample Spectrogram Images</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>259773</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="101" name="TextBox 100">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D998B1EA-4B31-488D-8269-E13C88E6A43B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16971818" y="36420135"/>
+          <a:ext cx="3896591" cy="4953001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> Accept bunch of Spectropgram Images as inputs</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>- Label each Image</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>- Construct CNN Layers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>- Be able to change the following parameters</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>0. Ratio between train and validate samples</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>1.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> Filter size in each layer</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>2. Epoch</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>3. Batch size</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>4. other parameters (currently</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> researching)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:br>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>Be able to plot the training and validation graph</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>277746</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>69636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>231322</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4AACAB4-69CB-4803-8133-3AC6097C2A06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14361139" y="38087993"/>
+          <a:ext cx="565897" cy="297757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Mukit </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>314885</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>121983</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>408215</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="102" name="TextBox 101">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3012B6A-D052-46C8-A9DA-594537DE5AB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4601135" y="38140340"/>
+          <a:ext cx="705651" cy="313446"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Mahdieh</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>266860</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>167607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>353786</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>154529</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="103" name="TextBox 102">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E486E07-87AC-4873-A595-03FB56D22DD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14350253" y="38566964"/>
+          <a:ext cx="699247" cy="367922"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Paween </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>331214</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>2240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>424544</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>125186</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="104" name="TextBox 103">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{378F87D6-5638-40D3-8714-CE0959502E71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4617464" y="38592097"/>
+          <a:ext cx="705651" cy="313446"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Rabiul</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4298,10 +4983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A403C48-F16A-4071-B8EA-3F4F6C55080D}">
-  <dimension ref="E2:AV123"/>
+  <dimension ref="E2:AV131"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B120" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J127" sqref="J127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4657,40 +5342,51 @@
     <row r="112" spans="7:7" ht="15.75">
       <c r="G112" s="4"/>
     </row>
-    <row r="113" spans="7:7" ht="15.75">
+    <row r="113" spans="6:7" ht="15.75">
       <c r="G113" s="4"/>
     </row>
-    <row r="114" spans="7:7" ht="46.5">
+    <row r="114" spans="6:7" ht="46.5">
       <c r="G114" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="7:7" ht="15.75">
+    <row r="115" spans="6:7" ht="15.75">
       <c r="G115" s="4"/>
     </row>
-    <row r="116" spans="7:7" ht="15.75">
+    <row r="116" spans="6:7" ht="15.75">
       <c r="G116" s="4"/>
     </row>
-    <row r="117" spans="7:7" ht="15.75">
+    <row r="117" spans="6:7" ht="15.75">
       <c r="G117" s="4"/>
     </row>
-    <row r="118" spans="7:7" ht="15.75">
+    <row r="118" spans="6:7" ht="15.75">
       <c r="G118" s="4"/>
     </row>
-    <row r="119" spans="7:7" ht="15.75">
+    <row r="119" spans="6:7" ht="15.75">
       <c r="G119" s="4"/>
     </row>
-    <row r="120" spans="7:7" ht="15.75">
+    <row r="120" spans="6:7" ht="15.75">
       <c r="G120" s="4"/>
     </row>
-    <row r="121" spans="7:7" ht="15.75">
+    <row r="121" spans="6:7" ht="15.75">
       <c r="G121" s="4"/>
     </row>
-    <row r="122" spans="7:7" ht="15.75">
+    <row r="122" spans="6:7" ht="15.75">
       <c r="G122" s="4"/>
     </row>
-    <row r="123" spans="7:7" ht="15.75">
+    <row r="123" spans="6:7" ht="15.75">
       <c r="G123" s="4"/>
+    </row>
+    <row r="124" spans="6:7" s="9" customFormat="1"/>
+    <row r="128" spans="6:7" ht="61.5">
+      <c r="F128" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="6:6" ht="33.75">
+      <c r="F131" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add flowchart to experiment design
</commit_message>
<xml_diff>
--- a/ExperimentDesign/CNNwithSTFT_ExperimentDesign.xlsx
+++ b/ExperimentDesign/CNNwithSTFT_ExperimentDesign.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FRA-UAS\semester2\CompInt\CompInt-Project-T3\ExperimentDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE325C6-C4EB-4355-BFD2-4E838B43AA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D62DCC5-3CB9-42BC-A4EB-E5D2528C6BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F4F0541-79DD-4112-8FFC-CE99E882B6FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3F4F0541-79DD-4112-8FFC-CE99E882B6FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment Design" sheetId="1" r:id="rId1"/>
+    <sheet name="FlowChart Diagram" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t xml:space="preserve">CNN with STFT Experiment Design </t>
   </si>
@@ -74,12 +75,21 @@
   <si>
     <t>2 Parts</t>
   </si>
+  <si>
+    <t>Flowchart Diagram of Program.</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Remarks : Variable Type TBA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +153,30 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -164,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -172,11 +206,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -188,6 +302,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4678,6 +4804,2586 @@
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>Rabiul</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3417CD5-2F9F-4B9D-807F-4AB86838435C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3657600" y="2428875"/>
+          <a:ext cx="3047999" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Create STFT</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> from input</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>( createSTFT.py )</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B781C754-D6C4-4C9F-BC91-80DAA2A39A64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3657600" y="2095500"/>
+          <a:ext cx="3048000" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Create Spectrogram from STFT</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>( createSpectrogram.py )</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC77006F-0A3F-4ADA-BCEC-B093DBC481AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7315200" y="2428875"/>
+          <a:ext cx="3048000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Create  Convolution Network</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>( construnctConvNet.py )</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C230F714-2DCB-43D3-9996-EC46DFA99E45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="3238500"/>
+          <a:ext cx="3048000" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Train Network</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>( trainNetwork.py )</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7378E6DD-5DDF-4D32-96A4-91DE50A03C24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="4191000"/>
+          <a:ext cx="3048000" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Classification and validation</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>( classify.py )</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A3AAA27-623D-485F-B406-B7CA767791A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="5143500"/>
+          <a:ext cx="3048000" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Plot Training and Validation Graph</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>( plotTrainAndValidGraph.py )</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>384175</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Oval 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91754CCA-F355-46B0-85BB-031AFB396C0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6886575" y="180975"/>
+          <a:ext cx="203200" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Oval 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5157772C-E0CE-4C97-9104-A2D044A9B2C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6915150" y="8343900"/>
+          <a:ext cx="203200" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>282576</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Connector: Elbow 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{999F0A7F-D6BD-4B03-85A0-73F545843F7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="4"/>
+          <a:endCxn id="2" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5318126" y="758825"/>
+          <a:ext cx="1533525" cy="1806575"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>282575</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Connector: Elbow 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1C1BF68-A5EA-426D-9DEF-D57C5C381811}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="4"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="7146925" y="736599"/>
+          <a:ext cx="1533525" cy="1851025"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{878814CE-B8D3-4C07-B967-293B4CF32714}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="3" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5181600" y="3000375"/>
+          <a:ext cx="0" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E349D36-ADF4-4A89-9029-26269FE96612}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="6" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7010400" y="5286375"/>
+          <a:ext cx="0" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8402C07-7CEC-4343-98A6-338DB1CDBB1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="2"/>
+          <a:endCxn id="7" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7010400" y="6429375"/>
+          <a:ext cx="0" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4BFAF5D-4CB9-467C-948B-43B049B3A87E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="2"/>
+          <a:endCxn id="9" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7010400" y="7572375"/>
+          <a:ext cx="6350" cy="771525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Connector: Elbow 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18319069-4877-49AC-891B-C03410946389}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="5" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7781925" y="3943350"/>
+          <a:ext cx="1809750" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Connector: Elbow 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F91AA58-770C-4933-AA6E-3ADAB8DB4B9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="5" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="4905375" y="4419600"/>
+          <a:ext cx="857250" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="TextBox 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28D90836-DF6F-4CFF-A851-8E3A76243210}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="8715375"/>
+          <a:ext cx="609600" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>END</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="TextBox 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD77AB4D-3365-46AE-9557-92D1D7C858CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705600" y="523875"/>
+          <a:ext cx="609600" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>START</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>481853</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>145677</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="Rectangle 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB89B63B-959B-4CA2-BED8-7A237B880785}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1692088" y="2868705"/>
+          <a:ext cx="3294530" cy="2173941"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>493058</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="TextBox 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F817B7D-68AB-4D81-A42A-CAEBF38F8E5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1098176" y="5390029"/>
+          <a:ext cx="1927412" cy="515471"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If one</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> function can cover all then only one function</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>493058</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>89646</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>481853</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="Connector: Elbow 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B1E5492-9167-4F31-B269-F38064214077}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="42" idx="1"/>
+          <a:endCxn id="45" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="1098176" y="3955675"/>
+          <a:ext cx="593912" cy="1692089"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 138491"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>605117</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>605116</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="TextBox 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{620F278C-466D-4751-B87C-75871F6D4008}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10892117" y="1389529"/>
+          <a:ext cx="4235823" cy="2476500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>createSTFT.py and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>createSpectrogram.py</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Input Parameters </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Input path : string</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>2. Output path : string</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>3. Window e.g. hamming Window Rect window, but we will construct window outside function and import to the function</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>4. Overlapped Value : int</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>5. Output</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Images file type : string</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Output</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0"/>
+            <a:t>1. Spectrogram</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t> Images of all Signals : images (PNG, JPG, ...) </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="TextBox 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42170041-908D-4375-B727-0BDA8E1B4C8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10892118" y="4123764"/>
+          <a:ext cx="4235823" cy="1456765"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>constructConvNet.py</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Input Parameters </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>None</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Output</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0"/>
+            <a:t>1. network</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="TextBox 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08B6C910-3D1C-43FC-84F3-CA9AA307939A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10892118" y="5838264"/>
+          <a:ext cx="4235823" cy="2218765"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>trainNetwork.py and classify.py </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Input Parameters</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1. network</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2. Spectrogram Images ( Var type : TBA) </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>3. trainingOptions ( Probably read from config file )</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>4. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Output</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1. Trained Network</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2. Classification Result</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>499783</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>107576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>163607</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>186017</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="Rectangle 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DCDDD65-648A-4ECE-B815-6C42B9252764}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3525371" y="5116605"/>
+          <a:ext cx="3294530" cy="2173941"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>246529</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="TextBox 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C159766-42F2-4275-A736-5793B79FA6FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7395882" y="6656294"/>
+          <a:ext cx="1927412" cy="515471"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>If one</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> function can cover all then only one function</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>163607</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>51547</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>493059</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="Connector: Elbow 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1821E44C-26C7-477B-B15B-7D098B69212A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="60" idx="3"/>
+          <a:endCxn id="61" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6819901" y="6203576"/>
+          <a:ext cx="1539687" cy="452718"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="TextBox 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D715AA6D-A323-4E3C-B368-7F566B98E0DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10892118" y="8247530"/>
+          <a:ext cx="4235823" cy="1524000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>plotTrainAndValidGraph.py</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Input Parameters</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>TBA</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Output </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Graph of training and Validation Result</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4985,7 +7691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A403C48-F16A-4071-B8EA-3F4F6C55080D}">
   <dimension ref="E2:AV131"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B120" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A101" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="J127" sqref="J127"/>
     </sheetView>
   </sheetViews>
@@ -5393,4 +8099,817 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7831EF4-D0E8-47EA-8B49-08180CE33F2A}">
+  <dimension ref="B2:U49"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB17" sqref="AB17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:21" ht="26.25">
+      <c r="E2" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" ht="26.25">
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="2:21" ht="26.25">
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="16"/>
+      <c r="S4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21">
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="19"/>
+    </row>
+    <row r="6" spans="2:21">
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="19"/>
+    </row>
+    <row r="7" spans="2:21">
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="19"/>
+    </row>
+    <row r="8" spans="2:21">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="19"/>
+    </row>
+    <row r="9" spans="2:21">
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="19"/>
+    </row>
+    <row r="10" spans="2:21">
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="19"/>
+    </row>
+    <row r="11" spans="2:21">
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="19"/>
+    </row>
+    <row r="12" spans="2:21">
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="19"/>
+    </row>
+    <row r="13" spans="2:21">
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="19"/>
+    </row>
+    <row r="14" spans="2:21">
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="19"/>
+    </row>
+    <row r="15" spans="2:21">
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="19"/>
+    </row>
+    <row r="16" spans="2:21">
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="19"/>
+    </row>
+    <row r="17" spans="2:16">
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="19"/>
+    </row>
+    <row r="18" spans="2:16">
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="19"/>
+    </row>
+    <row r="19" spans="2:16">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="19"/>
+    </row>
+    <row r="20" spans="2:16">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="19"/>
+    </row>
+    <row r="21" spans="2:16">
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="19"/>
+    </row>
+    <row r="22" spans="2:16">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="19"/>
+    </row>
+    <row r="23" spans="2:16">
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="19"/>
+    </row>
+    <row r="24" spans="2:16">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="19"/>
+    </row>
+    <row r="25" spans="2:16">
+      <c r="B25" s="17"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="19"/>
+    </row>
+    <row r="26" spans="2:16">
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="19"/>
+    </row>
+    <row r="27" spans="2:16">
+      <c r="B27" s="17"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="19"/>
+    </row>
+    <row r="28" spans="2:16">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="19"/>
+    </row>
+    <row r="29" spans="2:16">
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="19"/>
+    </row>
+    <row r="30" spans="2:16">
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="19"/>
+    </row>
+    <row r="31" spans="2:16">
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="19"/>
+    </row>
+    <row r="32" spans="2:16">
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="19"/>
+    </row>
+    <row r="33" spans="2:16">
+      <c r="B33" s="17"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="19"/>
+    </row>
+    <row r="34" spans="2:16">
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="19"/>
+    </row>
+    <row r="35" spans="2:16">
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="19"/>
+    </row>
+    <row r="36" spans="2:16">
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="19"/>
+    </row>
+    <row r="37" spans="2:16">
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="19"/>
+    </row>
+    <row r="38" spans="2:16">
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="19"/>
+    </row>
+    <row r="39" spans="2:16">
+      <c r="B39" s="17"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="19"/>
+    </row>
+    <row r="40" spans="2:16">
+      <c r="B40" s="17"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="19"/>
+    </row>
+    <row r="41" spans="2:16">
+      <c r="B41" s="17"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="19"/>
+    </row>
+    <row r="42" spans="2:16">
+      <c r="B42" s="17"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="19"/>
+    </row>
+    <row r="43" spans="2:16">
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="19"/>
+    </row>
+    <row r="44" spans="2:16">
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="19"/>
+    </row>
+    <row r="45" spans="2:16">
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="19"/>
+    </row>
+    <row r="46" spans="2:16">
+      <c r="B46" s="17"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="19"/>
+    </row>
+    <row r="47" spans="2:16">
+      <c r="B47" s="17"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="19"/>
+    </row>
+    <row r="48" spans="2:16">
+      <c r="B48" s="17"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="19"/>
+    </row>
+    <row r="49" spans="2:16">
+      <c r="B49" s="20"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="21"/>
+      <c r="O49" s="21"/>
+      <c r="P49" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update experiment_design and Readme file
</commit_message>
<xml_diff>
--- a/ExperimentDesign/CNNwithSTFT_ExperimentDesign.xlsx
+++ b/ExperimentDesign/CNNwithSTFT_ExperimentDesign.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FRA-UAS\semester2\CompInt\CompInt-Project-T3\ExperimentDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28971E79-ABDF-41FD-A19A-090FA543EA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C156334-F8F5-4B1F-A3C7-F6F34599C60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F4F0541-79DD-4112-8FFC-CE99E882B6FB}"/>
   </bookViews>
@@ -566,21 +566,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -601,12 +586,41 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FFD60093"/>
+      <color rgb="FFFF0000"/>
+      <color rgb="FFCE36D2"/>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FFD731BF"/>
+      <color rgb="FFFFC000"/>
+      <color rgb="FF70AD47"/>
+      <color rgb="FF4472C4"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1040,79 +1054,18 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>231321</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>106892</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>57942</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>97725</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19" descr="What tools are good for drawing neural network architecture diagrams? -  Quora">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F2A7925-DE38-48B3-86A9-0E8556FEC8E9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="15384730" y="7640301"/>
-          <a:ext cx="10130939" cy="4493560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>353785</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>52</xdr:col>
-      <xdr:colOff>554182</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>103909</xdr:rowOff>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>295645</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>552945</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1127,8 +1080,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="24851591" y="5576455"/>
-          <a:ext cx="4191000" cy="3602181"/>
+          <a:off x="28520571" y="7783286"/>
+          <a:ext cx="4228110" cy="3927516"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1556,8 +1509,8 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:stCxn id="17" idx="3"/>
-          <a:endCxn id="20" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1615,8 +1568,8 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:stCxn id="19" idx="3"/>
-          <a:endCxn id="20" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1674,8 +1627,8 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:stCxn id="15" idx="3"/>
-          <a:endCxn id="20" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1733,8 +1686,8 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:stCxn id="13" idx="3"/>
-          <a:endCxn id="20" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1771,16 +1724,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>57942</xdr:colOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>310154</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>102308</xdr:rowOff>
+      <xdr:rowOff>4548</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>155864</xdr:rowOff>
+      <xdr:colOff>353785</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>17937</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1792,14 +1745,15 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="20" idx="3"/>
+          <a:cxnSpLocks/>
+          <a:stCxn id="6" idx="3"/>
           <a:endCxn id="21" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="25515669" y="9887081"/>
-          <a:ext cx="2366604" cy="261374"/>
+          <a:off x="27252297" y="9733655"/>
+          <a:ext cx="1268274" cy="13389"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4399,7 +4353,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5096,6 +5050,50 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>353785</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>310154</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>294845</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CFF0168-A8C2-4F89-A168-352C2C04065E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15661821" y="8014607"/>
+          <a:ext cx="11590476" cy="3438095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7701,6 +7699,2331 @@
             <a:defRPr/>
           </a:pPr>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Cube 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BDD1371-651C-4F94-A8EE-CB68B2A632CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11106151" y="2476500"/>
+          <a:ext cx="476250" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="cube">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 42162"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000">
+            <a:alpha val="54902"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B0F0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>131174</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="25" name="Group 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{672EA12A-EB36-44FF-A53F-070AFB3FE7DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2438400" y="1333499"/>
+          <a:ext cx="1959974" cy="2886075"/>
+          <a:chOff x="4425450" y="1120499"/>
+          <a:chExt cx="1959974" cy="2886075"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="21" name="Cube 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC1C5415-EAA8-4AB0-8A0A-01E8A61B98EB}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4425450" y="1120499"/>
+            <a:ext cx="1080000" cy="2886075"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 74162"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="ED7D31">
+              <a:alpha val="63922"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent2">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent2"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Cube 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6DE83C9-1660-462F-9497-93C99878A691}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4714875" y="1123950"/>
+            <a:ext cx="1080000" cy="2880000"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 74162"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="4472C4">
+              <a:alpha val="65098"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="Cube 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D45D956-A425-4AFA-9FD8-42386BCCF93A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5006475" y="1120499"/>
+            <a:ext cx="1080000" cy="2886075"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 74162"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="70AD47">
+              <a:alpha val="65098"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Cube 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1E13061-35E7-49CA-A504-2416DD1D7A3F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5305424" y="1123950"/>
+            <a:ext cx="1080000" cy="2880000"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 74162"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000">
+              <a:alpha val="65098"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent4">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent4"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent4"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>498975</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>22201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>451350</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>22500</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="24" name="Group 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF1462C7-2EAE-4E32-AA92-48C22C339746}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4156575" y="1546201"/>
+          <a:ext cx="1781175" cy="2476799"/>
+          <a:chOff x="6715125" y="1333500"/>
+          <a:chExt cx="1781175" cy="2476799"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="Cube 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{378394CA-EC6C-4230-92E1-B2F83189BABA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6715125" y="1333500"/>
+            <a:ext cx="1080000" cy="2476500"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 50106"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="ED7D31">
+              <a:alpha val="54902"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent2">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent2"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="Cube 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9B60894-2430-4524-9CA5-DF7170254CE0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7258049" y="1343024"/>
+            <a:ext cx="762001" cy="2467275"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 69401"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="4472C4">
+              <a:alpha val="54902"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="20" name="Cube 19">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F2DDE41-27F2-4CA0-B315-29A850B0BCB4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7496174" y="1343024"/>
+            <a:ext cx="762001" cy="2467275"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 69401"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="70AD47">
+              <a:alpha val="54902"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="22" name="Cube 21">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A9D1841-B42A-4E78-AB6F-B7CDE8177C70}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7734299" y="1342725"/>
+            <a:ext cx="762001" cy="2467275"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 69401"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000">
+              <a:alpha val="54902"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent4">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent4"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent4"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>451350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>22500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>194176</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>32025</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="29" name="Group 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{423CBEC8-822C-4A06-9573-C58E27824304}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5937750" y="1737000"/>
+          <a:ext cx="2181226" cy="2105025"/>
+          <a:chOff x="7924800" y="1524000"/>
+          <a:chExt cx="2181226" cy="2105025"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="23" name="Cube 22">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBFB3B81-D1E9-4AF2-9D47-9324985D4B4D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7924800" y="1533525"/>
+            <a:ext cx="1371601" cy="2095500"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 27734"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="ED7D31">
+              <a:alpha val="74902"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent2">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent2"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="26" name="Cube 25">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B4732B7-7CC5-4685-97F7-5671E8B33786}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8915399" y="1524000"/>
+            <a:ext cx="676276" cy="2095500"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 58209"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="4472C4">
+              <a:alpha val="74902"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="27" name="Cube 26">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5C1F179-EB81-4386-80F9-7EA0FF06A8FB}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9144000" y="1524000"/>
+            <a:ext cx="676276" cy="2095500"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 58209"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="70AD47">
+              <a:alpha val="74902"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="28" name="Cube 27">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AD4ED72-5BEA-4D73-A920-A2D9257256C1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9429750" y="1524000"/>
+            <a:ext cx="676276" cy="2095500"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 58209"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000">
+              <a:alpha val="74902"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent4">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent4"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent4"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>53474</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>155850</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="30" name="Group 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82C65257-954C-481D-BEBE-ACA0781E3F36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7978274" y="2095500"/>
+          <a:ext cx="2384926" cy="1489350"/>
+          <a:chOff x="7924800" y="1524000"/>
+          <a:chExt cx="2181226" cy="2105025"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="31" name="Cube 30">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D6D0C18-EC51-4BCD-BE51-262C58ECFF82}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7924800" y="1533525"/>
+            <a:ext cx="1371601" cy="2095500"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 27734"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="ED7D31">
+              <a:alpha val="65098"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent2">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent2"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="32" name="Cube 31">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6E4224F-E6D4-4D31-98EE-1EE54E661917}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8915399" y="1524000"/>
+            <a:ext cx="676276" cy="2095500"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 58209"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="4472C4">
+              <a:alpha val="65098"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="33" name="Cube 32">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B86BF4EC-9B98-472D-935E-C0A8D1CB745E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9144000" y="1524000"/>
+            <a:ext cx="676276" cy="2095500"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 58209"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="70AD47">
+              <a:alpha val="65098"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="34" name="Cube 33">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0049AB8-DA68-48B7-BE74-57225A8AA7E8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9429750" y="1524000"/>
+            <a:ext cx="676276" cy="2095500"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 58209"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000">
+              <a:alpha val="65098"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent4">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent4"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent4"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="47" name="Group 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28792815-6C6D-48A8-A2C1-9BC933384F21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="10363200" y="2286000"/>
+          <a:ext cx="1828800" cy="1143000"/>
+          <a:chOff x="9144000" y="2286000"/>
+          <a:chExt cx="1828800" cy="1143000"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="Cube 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0294B3C6-9AE5-4E38-A634-C119D51B5B54}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9144000" y="2286000"/>
+            <a:ext cx="1097756" cy="1143000"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 22969"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="ED7D31">
+              <a:alpha val="54902"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent2">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent2"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="44" name="Cube 43">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32DE0626-B1B8-49B2-87BE-36AD060633C1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9991726" y="2286000"/>
+            <a:ext cx="495300" cy="1143000"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 50779"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="4472C4">
+              <a:alpha val="54902"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="45" name="Cube 44">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1956B488-AD6B-447B-BDDA-625BE1AC3DF8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10229850" y="2286000"/>
+            <a:ext cx="495300" cy="1143000"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 50779"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="70AD47">
+              <a:alpha val="54902"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="46" name="Cube 45">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13D8F2FD-32AF-4C19-80C2-302DC80E9E4B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10477500" y="2286000"/>
+            <a:ext cx="495300" cy="1143000"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 50779"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000">
+              <a:alpha val="54902"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent4">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent4"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent4"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>409576</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Cube 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B57966B-80E7-4BCE-8E85-85916520558B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11382376" y="2476500"/>
+          <a:ext cx="476250" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="cube">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 42162"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="D60093">
+            <a:alpha val="54902"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="Cube 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E803886D-6346-493F-B227-479488E10AE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11658601" y="2476500"/>
+          <a:ext cx="476250" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="cube">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 42162"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFCCFF">
+            <a:alpha val="54902"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="CE36D2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>181146</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>432299</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>5781</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Straight Arrow Connector 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53331E85-B2E8-4D99-9B3C-98001482E493}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="17" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2638425" y="3038646"/>
+          <a:ext cx="841874" cy="15135"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Straight Arrow Connector 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DD70E5F-55F8-4D0D-9820-FD953DD960CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4486275" y="2990850"/>
+          <a:ext cx="828675" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>410123</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>124077</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Straight Arrow Connector 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6091F27E-CAB0-435A-88C6-E7C4E9F378CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="28" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6506123" y="2981325"/>
+          <a:ext cx="809077" cy="252"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>305348</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>252</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>252</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="Straight Arrow Connector 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6E4EF8D-51AB-4F2B-8B90-4F9991172CAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8839748" y="2857752"/>
+          <a:ext cx="666202" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>362498</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38352</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38352</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Straight Arrow Connector 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B36A76B-5A4C-474B-BBB2-0E84381A0452}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10725698" y="2895852"/>
+          <a:ext cx="437602" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="76" name="TextBox 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66418B6D-F683-44F2-8FD2-E0672871B2E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2438400" y="4219575"/>
+          <a:ext cx="257175" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>8</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="77" name="TextBox 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABAE5E5B-6C5C-419D-9C37-3BA22BF08B6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4267200" y="4029075"/>
+          <a:ext cx="381000" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>16</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="78" name="TextBox 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0014E21F-BA73-4613-BB8B-8C7CDA015AB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6257925" y="3838575"/>
+          <a:ext cx="381000" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>32</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="79" name="TextBox 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CE65D7A-7B90-43A4-BA2C-9FE30EA6ECD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8429625" y="3571875"/>
+          <a:ext cx="438150" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>64</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="TextBox 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D07785E4-B99C-4DAA-A4B9-1881CC76F7F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10601324" y="3419475"/>
+          <a:ext cx="542925" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>128</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="106" name="Cube 105">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAC6B941-DC7A-4255-9C33-838DC401FC85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="5905500"/>
+          <a:ext cx="228600" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="cube">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 22969"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ED7D31">
+            <a:alpha val="54902"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="107" name="Cube 106">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0D209C4-E126-427D-97D1-5E78EEB1E3CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="5715000"/>
+          <a:ext cx="228600" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="cube">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 22969"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ED7D31">
+            <a:alpha val="54902"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="108" name="Cube 107">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D312062-EA43-41DE-8356-C7563EF1FA34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="5524500"/>
+          <a:ext cx="228600" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="cube">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 22969"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ED7D31">
+            <a:alpha val="54902"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="109" name="Cube 108">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{486880B4-6EDC-4EF4-9380-FAD21F0CFD2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="5334000"/>
+          <a:ext cx="228600" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="cube">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 22969"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ED7D31">
+            <a:alpha val="54902"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -8008,8 +10331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A403C48-F16A-4071-B8EA-3F4F6C55080D}">
   <dimension ref="E2:AV131"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17:AQ39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AQ36" sqref="AQ36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9242,7 +11565,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="42" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="37" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" customWidth="1"/>
@@ -9253,7 +11576,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25">
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="34" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="13"/>
@@ -9263,58 +11586,58 @@
       <c r="H1" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="30" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="30" t="s">
+      <c r="H3" s="41"/>
+      <c r="I3" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="38" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30">
-      <c r="A4" s="34"/>
-      <c r="B4" s="40" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="36" t="s">
+      <c r="F4" s="39"/>
+      <c r="G4" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:10" ht="60">
       <c r="A5" s="29">
         <v>1</v>
       </c>
-      <c r="B5" s="41" t="str">
+      <c r="B5" s="36" t="str">
         <f>PROPER(Window!A1)</f>
         <v>Barthannwin</v>
       </c>
@@ -9343,7 +11666,7 @@
       <c r="A6" s="29">
         <v>2</v>
       </c>
-      <c r="B6" s="41" t="str">
+      <c r="B6" s="36" t="str">
         <f>PROPER(Window!A2)</f>
         <v xml:space="preserve">Bartlett
 </v>
@@ -9373,7 +11696,7 @@
       <c r="A7" s="29">
         <v>3</v>
       </c>
-      <c r="B7" s="41" t="str">
+      <c r="B7" s="36" t="str">
         <f>PROPER(Window!A3)</f>
         <v xml:space="preserve">Blackman
 </v>
@@ -9403,7 +11726,7 @@
       <c r="A8" s="29">
         <v>4</v>
       </c>
-      <c r="B8" s="41" t="str">
+      <c r="B8" s="36" t="str">
         <f>PROPER(Window!A4)</f>
         <v xml:space="preserve">Blackmanharris
 </v>
@@ -9433,7 +11756,7 @@
       <c r="A9" s="29">
         <v>5</v>
       </c>
-      <c r="B9" s="41" t="str">
+      <c r="B9" s="36" t="str">
         <f>PROPER(Window!A5)</f>
         <v xml:space="preserve">Bohmanwin
 </v>
@@ -9463,7 +11786,7 @@
       <c r="A10" s="29">
         <v>6</v>
       </c>
-      <c r="B10" s="41" t="str">
+      <c r="B10" s="36" t="str">
         <f>PROPER(Window!A6)</f>
         <v xml:space="preserve">Chebwin
 </v>
@@ -9493,7 +11816,7 @@
       <c r="A11" s="29">
         <v>7</v>
       </c>
-      <c r="B11" s="41" t="str">
+      <c r="B11" s="36" t="str">
         <f>PROPER(Window!A7)</f>
         <v xml:space="preserve">Flattopwin
 </v>
@@ -9523,7 +11846,7 @@
       <c r="A12" s="29">
         <v>8</v>
       </c>
-      <c r="B12" s="41" t="str">
+      <c r="B12" s="36" t="str">
         <f>PROPER(Window!A8)</f>
         <v xml:space="preserve">Gausswin
 </v>
@@ -9553,7 +11876,7 @@
       <c r="A13" s="29">
         <v>9</v>
       </c>
-      <c r="B13" s="41" t="str">
+      <c r="B13" s="36" t="str">
         <f>PROPER(Window!A9)</f>
         <v xml:space="preserve">Hamming
 </v>
@@ -9577,7 +11900,7 @@
         <v>51</v>
       </c>
       <c r="I13" s="23"/>
-      <c r="J13" s="37" t="s">
+      <c r="J13" s="32" t="s">
         <v>52</v>
       </c>
     </row>
@@ -9585,7 +11908,7 @@
       <c r="A14" s="29">
         <v>10</v>
       </c>
-      <c r="B14" s="41" t="str">
+      <c r="B14" s="36" t="str">
         <f>PROPER(Window!A10)</f>
         <v xml:space="preserve">Hann
 </v>
@@ -9615,7 +11938,7 @@
       <c r="A15" s="29">
         <v>11</v>
       </c>
-      <c r="B15" s="41" t="str">
+      <c r="B15" s="36" t="str">
         <f>PROPER(Window!A11)</f>
         <v xml:space="preserve">Kaiser
 </v>
@@ -9645,7 +11968,7 @@
       <c r="A16" s="29">
         <v>12</v>
       </c>
-      <c r="B16" s="41" t="str">
+      <c r="B16" s="36" t="str">
         <f>PROPER(Window!A12)</f>
         <v xml:space="preserve">Nuttallwin
 </v>
@@ -9675,7 +11998,7 @@
       <c r="A17" s="29">
         <v>13</v>
       </c>
-      <c r="B17" s="41" t="str">
+      <c r="B17" s="36" t="str">
         <f>PROPER(Window!A13)</f>
         <v xml:space="preserve">Parzenwin
 </v>
@@ -9705,7 +12028,7 @@
       <c r="A18" s="29">
         <v>14</v>
       </c>
-      <c r="B18" s="41" t="str">
+      <c r="B18" s="36" t="str">
         <f>PROPER(Window!A14)</f>
         <v xml:space="preserve">Rectwin
 </v>
@@ -9735,7 +12058,7 @@
       <c r="A19" s="29">
         <v>15</v>
       </c>
-      <c r="B19" s="41" t="str">
+      <c r="B19" s="36" t="str">
         <f>PROPER(Window!A15)</f>
         <v xml:space="preserve">Taylorwin
 </v>
@@ -9765,7 +12088,7 @@
       <c r="A20" s="29">
         <v>16</v>
       </c>
-      <c r="B20" s="41" t="str">
+      <c r="B20" s="36" t="str">
         <f>PROPER(Window!A16)</f>
         <v xml:space="preserve">Triang
 </v>
@@ -9795,7 +12118,7 @@
       <c r="A21" s="29">
         <v>17</v>
       </c>
-      <c r="B21" s="41" t="str">
+      <c r="B21" s="36" t="str">
         <f>PROPER(Window!A17)</f>
         <v xml:space="preserve">Tukeywin
 </v>
@@ -9840,8 +12163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C85610-A4C9-4EBC-9DAF-5135C98C1310}">
   <dimension ref="B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9853,6 +12176,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9867,87 +12191,87 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1" ht="30">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="33" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="30">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="33" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="45">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="33" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="45">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="33" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="45">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="33" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="30">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="33" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="45">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="33" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="30">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="33" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="45">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="33" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="30">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="33" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="30">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="45">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="33" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="45">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="33" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="30">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="33" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="45">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="33" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="30">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="33" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="45">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="33" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
filter non-necessary info from design
</commit_message>
<xml_diff>
--- a/ExperimentDesign/CNNwithSTFT_ExperimentDesign.xlsx
+++ b/ExperimentDesign/CNNwithSTFT_ExperimentDesign.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FRA-UAS\semester2\CompInt\CompInt-Project-T3\ExperimentDesign\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\FRA-UAS\semester2\CompInt\Classification-of-time-signals-by-CNN-using-STFT\ExperimentDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E0BB52-80B6-475C-9045-BC55EEC98505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0F0084-2AF1-48CC-93CB-4D8F4311EEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{3F4F0541-79DD-4112-8FFC-CE99E882B6FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F4F0541-79DD-4112-8FFC-CE99E882B6FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment Design" sheetId="1" r:id="rId1"/>
     <sheet name="FlowChart Diagram of Program" sheetId="2" r:id="rId2"/>
-    <sheet name="Experiment Prarameters" sheetId="4" r:id="rId3"/>
-    <sheet name="CNN Model 1" sheetId="5" r:id="rId4"/>
-    <sheet name="CNN Model 2" sheetId="8" r:id="rId5"/>
-    <sheet name="drawing" sheetId="9" r:id="rId6"/>
-    <sheet name="Window" sheetId="7" r:id="rId7"/>
+    <sheet name="Experiment Prarameters" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="CNN Model 1" sheetId="5" state="hidden" r:id="rId4"/>
+    <sheet name="CNN Model 2" sheetId="8" state="hidden" r:id="rId5"/>
+    <sheet name="drawing" sheetId="9" state="hidden" r:id="rId6"/>
+    <sheet name="Window" sheetId="7" state="hidden" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -527,6 +527,8 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -542,8 +544,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7355,50 +7355,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>585476</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>151286</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C326B3B-AE18-41DD-A6F4-3183F626BD0D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16532679" y="1401536"/>
-          <a:ext cx="7933333" cy="8914286"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -13883,9 +13839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A403C48-F16A-4071-B8EA-3F4F6C55080D}">
   <dimension ref="E2:AV131"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -14297,9 +14251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7831EF4-D0E8-47EA-8B49-08180CE33F2A}">
   <dimension ref="B2:U49"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -14312,7 +14264,7 @@
       <c r="E3" s="13"/>
     </row>
     <row r="4" spans="2:21" ht="26.25">
-      <c r="B4" s="36"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -15138,31 +15090,31 @@
       <c r="H1" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="30" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="30" t="s">
+      <c r="H3" s="35"/>
+      <c r="I3" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30">
-      <c r="A4" s="31"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="27" t="s">
         <v>22</v>
       </c>
@@ -15175,15 +15127,15 @@
       <c r="E4" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="31"/>
+      <c r="F4" s="33"/>
       <c r="G4" s="23" t="s">
         <v>48</v>
       </c>
       <c r="H4" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="60">
       <c r="A5" s="21">
@@ -15727,42 +15679,42 @@
       </c>
     </row>
     <row r="26" spans="9:13" ht="15.75">
-      <c r="I26" s="35" t="s">
+      <c r="I26" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="M26" s="35" t="s">
+      <c r="M26" s="30" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="27" spans="9:13" ht="15.75">
-      <c r="I27" s="35"/>
-      <c r="M27" s="35"/>
+      <c r="I27" s="30"/>
+      <c r="M27" s="30"/>
     </row>
     <row r="28" spans="9:13" ht="15.75">
-      <c r="I28" s="35" t="s">
+      <c r="I28" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="M28" s="35" t="s">
+      <c r="M28" s="30" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="9:13" ht="15.75">
-      <c r="I29" s="35"/>
-      <c r="M29" s="35"/>
+      <c r="I29" s="30"/>
+      <c r="M29" s="30"/>
     </row>
     <row r="30" spans="9:13" ht="15.75">
-      <c r="I30" s="35" t="s">
+      <c r="I30" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="M30" s="35" t="s">
+      <c r="M30" s="30" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="9:13" ht="15.75">
-      <c r="I31" s="35"/>
+      <c r="I31" s="30"/>
     </row>
     <row r="32" spans="9:13" ht="15.75">
-      <c r="I32" s="35" t="s">
+      <c r="I32" s="30" t="s">
         <v>57</v>
       </c>
     </row>
@@ -15788,42 +15740,42 @@
   </cols>
   <sheetData>
     <row r="25" spans="7:11" ht="15.75">
-      <c r="G25" s="35" t="s">
+      <c r="G25" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="K25" s="35" t="s">
+      <c r="K25" s="30" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="26" spans="7:11" ht="15.75">
-      <c r="G26" s="35"/>
-      <c r="K26" s="35"/>
+      <c r="G26" s="30"/>
+      <c r="K26" s="30"/>
     </row>
     <row r="27" spans="7:11" ht="15.75">
-      <c r="G27" s="35" t="s">
+      <c r="G27" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K27" s="35" t="s">
+      <c r="K27" s="30" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="28" spans="7:11" ht="15.75">
-      <c r="G28" s="35"/>
-      <c r="K28" s="35"/>
+      <c r="G28" s="30"/>
+      <c r="K28" s="30"/>
     </row>
     <row r="29" spans="7:11" ht="15.75">
-      <c r="G29" s="35" t="s">
+      <c r="G29" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="K29" s="35" t="s">
+      <c r="K29" s="30" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="30" spans="7:11" ht="15.75">
-      <c r="G30" s="35"/>
+      <c r="G30" s="30"/>
     </row>
     <row r="31" spans="7:11" ht="15.75">
-      <c r="G31" s="35" t="s">
+      <c r="G31" s="30" t="s">
         <v>57</v>
       </c>
     </row>
@@ -15837,7 +15789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445E038D-E302-4ED4-80E0-AE5510D91AA3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>

</xml_diff>